<commit_message>
multi changes of About page
</commit_message>
<xml_diff>
--- a/R1/assets/data/ICAST_IOC Committee_2025.xlsx
+++ b/R1/assets/data/ICAST_IOC Committee_2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STVL LAB\ICAST2026 website\ICAST2026-website\R1\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A31413-E609-413F-9B9E-2439E6C05186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118C5B7C-5449-484D-A1FB-872D438D5D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{21A00F37-F168-469C-B495-5B188FB1F7DD}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
   <si>
     <t>IOC Member</t>
   </si>
@@ -159,9 +159,6 @@
     <t xml:space="preserve">Hiroaki Tanaka &lt;tanakah@nda.ac.jp&gt;; </t>
   </si>
   <si>
-    <t>H. Wang, Chongqing University, China</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dai-Hua Wang &lt;dhwang@cqu.edu.cn&gt;; </t>
   </si>
   <si>
@@ -204,9 +201,6 @@
     <t>Kazuyuki HANAHARA &lt;hanahara@iwate-u.ac.jp&gt;;</t>
   </si>
   <si>
-    <t>K. Lee, National Taiwan University, Taiwan</t>
-  </si>
-  <si>
     <t>cklee@ntu.edu.tw;</t>
   </si>
   <si>
@@ -261,118 +255,138 @@
     <t xml:space="preserve">Paolo Gaudenzi &lt;paolo.gaudenzi@uniroma1.it&gt;; </t>
   </si>
   <si>
+    <t>R.DeBreuker@tudelft.nl;</t>
+  </si>
+  <si>
+    <t>R. Ohayon, Conservatoire National des Arts et Métiers, France</t>
+  </si>
+  <si>
+    <t>Roger Ohayon &lt;roger.ohayon@lecnam.net&gt;;</t>
+  </si>
+  <si>
+    <t>Roger Ohayon &lt;roger.ohayon@cnam.fr&gt;;</t>
+  </si>
+  <si>
+    <t>W. H. Liao, Chinese University of Hong Kong, China</t>
+  </si>
+  <si>
+    <t>Wei Hsin Liao (MAEG) &lt;whliao@cuhk.edu.hk&gt;;</t>
+  </si>
+  <si>
+    <t>W. J. Staszewski, AGH University of Science &amp; Technology, Poland</t>
+  </si>
+  <si>
+    <t>staszews@agh.edu.pl;</t>
+  </si>
+  <si>
+    <t>W.-J. Wu, National Taiwan University, Taiwan</t>
+  </si>
+  <si>
+    <t>Wen-Jong Wu &lt;wjwu@ntu.edu.tw&gt;;</t>
+  </si>
+  <si>
+    <t>X. X. Jiang, Canadian Space Agency, Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xinxiangjiang@cunet.carleton.ca; </t>
+  </si>
+  <si>
+    <t>Y. Chen, National Research Council, Canada</t>
+  </si>
+  <si>
+    <t>Eric &lt;Eric.Chen@nrc-cnrc.gc.ca&gt;;</t>
+  </si>
+  <si>
+    <t>Z. Gurdal, University of South Carolina, USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gurdal@cec.sc.edu; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">zgurdal@skoltech.ru; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramin Sedaghati &lt;ramin.sedaghati@concordia.ca&gt;; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mfanz@nuaa.edu.cn; </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>M. Fan, Nanjing University of Aeronautics and Astronautics, China</t>
+  </si>
+  <si>
+    <t>zbyang@ust.hk</t>
+  </si>
+  <si>
+    <t>liangjr@shanghaitech.edu.cn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TZOU, Hornsen &lt;hstzou@nuaa.edu.cn&gt;; </t>
+  </si>
+  <si>
+    <t>qiu@nuaa.edu.cn</t>
+  </si>
+  <si>
+    <t>jiong.tang@uconn.edu</t>
+  </si>
+  <si>
+    <t>J.Jovanova@tudelft.nl</t>
+  </si>
+  <si>
+    <t>flavio.campanile@dlr.de</t>
+  </si>
+  <si>
+    <t>permanni@ethz.ch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nsgoo@konkuk.ac.kr </t>
+  </si>
+  <si>
+    <t>C. K. Lee, National Taiwan University, Taiwan</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>suyili@vt.edu</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Z. B. Yang, Hong Kong University of Science and Technology, Hong Kong</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>J. R. Liang, ShanghaiTech University, China</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>J. Tang,  University of Connecticut, USA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>S. Y. Li, Virginia Tech, USA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>J. Jovanova, Univ. of Delft, Netherlands</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>R. Sedaghati, Concordia University, Canada</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D. H. Wang, Chongqing University, China</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>last name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>R. De Breuker, Delft University of Technology, Netherlands</t>
-  </si>
-  <si>
-    <t>R.DeBreuker@tudelft.nl;</t>
-  </si>
-  <si>
-    <t>R. Ohayon, Conservatoire National des Arts et Métiers, France</t>
-  </si>
-  <si>
-    <t>Roger Ohayon &lt;roger.ohayon@lecnam.net&gt;;</t>
-  </si>
-  <si>
-    <t>Roger Ohayon &lt;roger.ohayon@cnam.fr&gt;;</t>
-  </si>
-  <si>
-    <t>W. H. Liao, Chinese University of Hong Kong, China</t>
-  </si>
-  <si>
-    <t>Wei Hsin Liao (MAEG) &lt;whliao@cuhk.edu.hk&gt;;</t>
-  </si>
-  <si>
-    <t>W. J. Staszewski, AGH University of Science &amp; Technology, Poland</t>
-  </si>
-  <si>
-    <t>staszews@agh.edu.pl;</t>
-  </si>
-  <si>
-    <t>W.-J. Wu, National Taiwan University, Taiwan</t>
-  </si>
-  <si>
-    <t>Wen-Jong Wu &lt;wjwu@ntu.edu.tw&gt;;</t>
-  </si>
-  <si>
-    <t>X. X. Jiang, Canadian Space Agency, Canada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xinxiangjiang@cunet.carleton.ca; </t>
-  </si>
-  <si>
-    <t>Y. Chen, National Research Council, Canada</t>
-  </si>
-  <si>
-    <t>Eric &lt;Eric.Chen@nrc-cnrc.gc.ca&gt;;</t>
-  </si>
-  <si>
-    <t>Z. Gurdal, University of South Carolina, USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gurdal@cec.sc.edu; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">zgurdal@skoltech.ru; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ramin Sedaghati &lt;ramin.sedaghati@concordia.ca&gt;; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mfanz@nuaa.edu.cn; </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>M. Fan, Nanjing University of Aeronautics and Astronautics, China</t>
-  </si>
-  <si>
-    <t>R. Sedaghati, Concordia University, CAN</t>
-  </si>
-  <si>
-    <t>zbyang@ust.hk</t>
-  </si>
-  <si>
-    <t>liangjr@shanghaitech.edu.cn</t>
-  </si>
-  <si>
-    <t>Z. Yang, Hong Kong University of Science and Technology</t>
-  </si>
-  <si>
-    <t>J. Liang, ShanghaiTech University</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TZOU, Hornsen &lt;hstzou@nuaa.edu.cn&gt;; </t>
-  </si>
-  <si>
-    <t>qiu@nuaa.edu.cn</t>
-  </si>
-  <si>
-    <t>jiong.tang@uconn.edu</t>
-  </si>
-  <si>
-    <t>J. Tang,  University of Connecticut</t>
-  </si>
-  <si>
-    <t>S. Li, Virginia Tech</t>
-  </si>
-  <si>
-    <t>suyili@vt.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> J. Jovanova (Univ. of Delft)</t>
-  </si>
-  <si>
-    <t>J.Jovanova@tudelft.nl</t>
-  </si>
-  <si>
-    <t>flavio.campanile@dlr.de</t>
-  </si>
-  <si>
-    <t>permanni@ethz.ch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nsgoo@konkuk.ac.kr </t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -429,7 +443,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -478,12 +492,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -511,6 +543,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -842,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F19923-FAAE-4C42-B64A-CDC3A4E882B2}">
-  <dimension ref="B1:C62"/>
+  <dimension ref="B1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -855,522 +899,743 @@
     <col min="4" max="7" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B2, FIND(",",B2) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Abramovich</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+      <c r="D3" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B3, FIND(",",B3) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Bergamini</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B4, FIND(",",B4) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Brei</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B5, FIND(",",B5) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Campanile</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B6, FIND(",",B6) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Chen</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B7, FIND(",",B7) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Chopra</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B8, FIND(",",B8) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Collet</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="D9" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B9, FIND(",",B9) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Concilio</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B10, FIND(",",B10) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Breuker</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B11, FIND(",",B11) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Deü</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B12, FIND(",",B12) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Dragoni</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B13, FIND(",",B13) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Ermanni</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="10"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
+      <c r="D14" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B14, FIND(",",B14) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Erturk</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="14"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B16, FIND(",",B16) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Fan</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
+      <c r="D17" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B17, FIND(",",B17) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Flatau</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B18, FIND(",",B18) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Gandhi</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B19, FIND(",",B19) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Gaudenzi</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B20, FIND(",",B20) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Goo</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B21, FIND(",",B21) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Gurdal</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="12"/>
+      <c r="C22" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" s="7" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B23, FIND(",",B23) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Han</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B24, FIND(",",B24) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Hanahara</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B25, FIND(",",B25) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Hanselka</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B26, FIND(",",B26) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Inman</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B27, FIND(",",B27) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Jiang</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B28, FIND(",",B28) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Jovanova</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B29, FIND(",",B29) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Lagoudas</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B30, FIND(",",B30) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Lee</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B31, FIND(",",B31) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Lee</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B32, FIND(",",B32) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Leng</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B33, FIND(",",B33) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Lesieutre</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="12"/>
+      <c r="C34" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B35, FIND(",",B35) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Li</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B36, FIND(",",B36) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Liang</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B37, FIND(",",B37) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Liao</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B38, FIND(",",B38) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Martinez</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B39, FIND(",",B39) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Monner</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B40, FIND(",",B40) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Natori</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B41, FIND(",",B41) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Nitzsche</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="12"/>
+      <c r="C42" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B43, FIND(",",B43) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Ohayon</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="12"/>
+      <c r="C44" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B45, FIND(",",B45) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Okubo</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B46, FIND(",",B46) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Qiu</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B47, FIND(",",B47) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Saravanos</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B48, FIND(",",B48) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Sedaghati</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B49, FIND(",",B49) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Staszewski</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B50, FIND(",",B50) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Tanaka</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B51, FIND(",",B51) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Tang</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B52, FIND(",",B52) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Trindade</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B53, FIND(",",B53) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Tzou</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B54, FIND(",",B54) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Wang</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B55, FIND(",",B55) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Wang</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D56" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B56, FIND(",",B56) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Wereley</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
+      <c r="D57" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B57, FIND(",",B57) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Wickenheiser</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="10"/>
-      <c r="C16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="10"/>
-      <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" s="7" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="D58" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B58, FIND(",",B58) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Woods</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B59, FIND(",",B59) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Wu</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="10"/>
-      <c r="C47" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="10"/>
-      <c r="C55" s="2" t="s">
+      <c r="D60" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(LEFT(B60, FIND(",",B60) -1), " ",REPT(" ",100)), 100))</f>
+        <v>Yang</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="56" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B62" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="C62" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D60">
+    <sortCondition ref="D2:D60"/>
+  </sortState>
   <mergeCells count="5">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C29" r:id="rId1" xr:uid="{A97E2AFF-E202-4227-80DC-6B97067DF1C6}"/>
-    <hyperlink ref="C19" r:id="rId2" xr:uid="{072ED33C-DE0D-4EF0-BE8E-078D0B24DAC9}"/>
-    <hyperlink ref="C7" r:id="rId3" xr:uid="{9CE0E5B3-32C8-4007-AFB1-F867EBF37B6E}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{16E7D522-7002-4F12-9D67-6432736D63D0}"/>
-    <hyperlink ref="C33" r:id="rId5" xr:uid="{3F89F272-308D-4FAC-8F45-6FD76FC65615}"/>
-    <hyperlink ref="C9" r:id="rId6" display="mailto:drdiannbrei@umich.edu" xr:uid="{DA46CAE3-C477-4F6D-9415-5A115DAAB3D1}"/>
-    <hyperlink ref="C14" r:id="rId7" xr:uid="{1727C79B-DED6-4FA7-AA72-CEF279873094}"/>
-    <hyperlink ref="C42" r:id="rId8" xr:uid="{9D284668-5A9B-4E29-BDFB-728746B61B7C}"/>
-    <hyperlink ref="C20" r:id="rId9" xr:uid="{E0386201-9CE2-469E-A1A4-980973F15AD1}"/>
-    <hyperlink ref="C30" r:id="rId10" xr:uid="{1A48930B-64EC-4108-B685-8394A8AB1AC2}"/>
-    <hyperlink ref="C34" r:id="rId11" xr:uid="{0172E9BA-8657-4AA8-8F3D-766E059AF50E}"/>
-    <hyperlink ref="C27" r:id="rId12" xr:uid="{AE089A9E-3E37-4849-98E1-4C70BBF1CCC7}"/>
-    <hyperlink ref="C37" r:id="rId13" xr:uid="{8EEAA411-E580-4DDA-9298-6CD91BD9645B}"/>
-    <hyperlink ref="C36" r:id="rId14" xr:uid="{10C92037-12B5-4D42-A5E0-6CA49945F45E}"/>
-    <hyperlink ref="C21" r:id="rId15" xr:uid="{61FA2327-21AC-4C2D-A106-6D093629F2DD}"/>
-    <hyperlink ref="C35" r:id="rId16" xr:uid="{6C51C4D7-CABE-4AB7-B9FA-859011931510}"/>
-    <hyperlink ref="C45" r:id="rId17" xr:uid="{84CC406D-74F5-4477-87C4-FB25FF109CCF}"/>
-    <hyperlink ref="C12" r:id="rId18" xr:uid="{473EB45A-E09A-4889-9225-6EB831801D4E}"/>
-    <hyperlink ref="C50" r:id="rId19" xr:uid="{17EB55BC-BCAB-49A4-9D5E-CBB12C8F2C9E}"/>
-    <hyperlink ref="C52" r:id="rId20" xr:uid="{3ADEBEE9-1BB2-4DB2-B2F3-FD6875968BDB}"/>
-    <hyperlink ref="C54" r:id="rId21" xr:uid="{920E6D8A-6EEE-4ABF-A1DC-759D4FE67228}"/>
-    <hyperlink ref="C55" r:id="rId22" display="mailto:zgurdal@skoltech.ru" xr:uid="{DA82B581-6307-4B55-8AAF-CB6C09515110}"/>
-    <hyperlink ref="C38" r:id="rId23" xr:uid="{C6D4C68F-1EEE-4E0A-98B5-EE09DC0265E0}"/>
-    <hyperlink ref="C28" r:id="rId24" xr:uid="{53EFDB3B-939C-4E43-8F43-1F3E1C0E7385}"/>
-    <hyperlink ref="C58" r:id="rId25" xr:uid="{46F06B32-B111-44B2-B5AE-123942D3E9CB}"/>
-    <hyperlink ref="C56" r:id="rId26" xr:uid="{10C31905-C8AA-4C5D-9E80-89937212A690}"/>
-    <hyperlink ref="C57" r:id="rId27" xr:uid="{FA652201-90B8-4941-B865-27D79F3ED2FF}"/>
-    <hyperlink ref="C59" r:id="rId28" xr:uid="{7CDB6901-910F-45D0-AC9E-C74F1E612FBF}"/>
-    <hyperlink ref="C43" r:id="rId29" xr:uid="{792E263B-B14F-40F4-82A0-D54B28328BCA}"/>
-    <hyperlink ref="C60" r:id="rId30" xr:uid="{FD6C8B17-974F-486C-8D09-F8768A90692F}"/>
+    <hyperlink ref="C32" r:id="rId1" xr:uid="{A97E2AFF-E202-4227-80DC-6B97067DF1C6}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{072ED33C-DE0D-4EF0-BE8E-078D0B24DAC9}"/>
+    <hyperlink ref="C57" r:id="rId3" xr:uid="{9CE0E5B3-32C8-4007-AFB1-F867EBF37B6E}"/>
+    <hyperlink ref="C58" r:id="rId4" xr:uid="{16E7D522-7002-4F12-9D67-6432736D63D0}"/>
+    <hyperlink ref="C31" r:id="rId5" xr:uid="{3F89F272-308D-4FAC-8F45-6FD76FC65615}"/>
+    <hyperlink ref="C4" r:id="rId6" display="mailto:drdiannbrei@umich.edu" xr:uid="{DA46CAE3-C477-4F6D-9415-5A115DAAB3D1}"/>
+    <hyperlink ref="C18" r:id="rId7" xr:uid="{1727C79B-DED6-4FA7-AA72-CEF279873094}"/>
+    <hyperlink ref="C20" r:id="rId8" xr:uid="{9D284668-5A9B-4E29-BDFB-728746B61B7C}"/>
+    <hyperlink ref="C25" r:id="rId9" xr:uid="{E0386201-9CE2-469E-A1A4-980973F15AD1}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{1A48930B-64EC-4108-B685-8394A8AB1AC2}"/>
+    <hyperlink ref="C55" r:id="rId11" xr:uid="{0172E9BA-8657-4AA8-8F3D-766E059AF50E}"/>
+    <hyperlink ref="C30" r:id="rId12" xr:uid="{AE089A9E-3E37-4849-98E1-4C70BBF1CCC7}"/>
+    <hyperlink ref="C8" r:id="rId13" xr:uid="{8EEAA411-E580-4DDA-9298-6CD91BD9645B}"/>
+    <hyperlink ref="C40" r:id="rId14" xr:uid="{10C92037-12B5-4D42-A5E0-6CA49945F45E}"/>
+    <hyperlink ref="C45" r:id="rId15" xr:uid="{61FA2327-21AC-4C2D-A106-6D093629F2DD}"/>
+    <hyperlink ref="C5" r:id="rId16" xr:uid="{6C51C4D7-CABE-4AB7-B9FA-859011931510}"/>
+    <hyperlink ref="C10" r:id="rId17" xr:uid="{84CC406D-74F5-4477-87C4-FB25FF109CCF}"/>
+    <hyperlink ref="C47" r:id="rId18" xr:uid="{473EB45A-E09A-4889-9225-6EB831801D4E}"/>
+    <hyperlink ref="C49" r:id="rId19" xr:uid="{17EB55BC-BCAB-49A4-9D5E-CBB12C8F2C9E}"/>
+    <hyperlink ref="C27" r:id="rId20" xr:uid="{3ADEBEE9-1BB2-4DB2-B2F3-FD6875968BDB}"/>
+    <hyperlink ref="C21" r:id="rId21" xr:uid="{920E6D8A-6EEE-4ABF-A1DC-759D4FE67228}"/>
+    <hyperlink ref="C22" r:id="rId22" display="mailto:zgurdal@skoltech.ru" xr:uid="{DA82B581-6307-4B55-8AAF-CB6C09515110}"/>
+    <hyperlink ref="C16" r:id="rId23" xr:uid="{C6D4C68F-1EEE-4E0A-98B5-EE09DC0265E0}"/>
+    <hyperlink ref="C46" r:id="rId24" xr:uid="{53EFDB3B-939C-4E43-8F43-1F3E1C0E7385}"/>
+    <hyperlink ref="C51" r:id="rId25" xr:uid="{46F06B32-B111-44B2-B5AE-123942D3E9CB}"/>
+    <hyperlink ref="C60" r:id="rId26" xr:uid="{10C31905-C8AA-4C5D-9E80-89937212A690}"/>
+    <hyperlink ref="C36" r:id="rId27" xr:uid="{FA652201-90B8-4941-B865-27D79F3ED2FF}"/>
+    <hyperlink ref="C35" r:id="rId28" xr:uid="{7CDB6901-910F-45D0-AC9E-C74F1E612FBF}"/>
+    <hyperlink ref="C13" r:id="rId29" xr:uid="{792E263B-B14F-40F4-82A0-D54B28328BCA}"/>
+    <hyperlink ref="C28" r:id="rId30" xr:uid="{FD6C8B17-974F-486C-8D09-F8768A90692F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
@@ -1378,6 +1643,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -1385,15 +1659,6 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1667,6 +1932,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F4B3-D335-4F30-B53B-EE2A82E50F0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{711F793D-6BE6-4EB4-A5EC-4719724D39C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1680,14 +1953,6 @@
     <ds:schemaRef ds:uri="04f307b9-a7a6-46a1-b058-6a05536458f4"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F4B3-D335-4F30-B53B-EE2A82E50F0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>